<commit_message>
Organisational practices reliability (not to use)
</commit_message>
<xml_diff>
--- a/Results/org_practices_reliability.xlsx
+++ b/Results/org_practices_reliability.xlsx
@@ -94,7 +94,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6783414012585154</v>
+        <v>0.6182220821905557</v>
       </c>
     </row>
     <row r="3">
@@ -102,7 +102,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.8248597442390206</v>
+        <v>0.8222533184040642</v>
       </c>
     </row>
     <row r="4">
@@ -110,7 +110,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.7049929769481568</v>
+        <v>0.6894054741978975</v>
       </c>
     </row>
     <row r="5">
@@ -118,7 +118,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.7049929769481568</v>
+        <v>0.6894054741978975</v>
       </c>
     </row>
     <row r="6">
@@ -126,7 +126,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.7049929793567923</v>
+        <v>0.6894054762660493</v>
       </c>
     </row>
     <row r="7">
@@ -134,7 +134,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.6387423381325241</v>
+        <v>0.6345773421346755</v>
       </c>
     </row>
   </sheetData>

</xml_diff>